<commit_message>
updated analysis and ML
</commit_message>
<xml_diff>
--- a/BRFSS_Field_Map.xlsx
+++ b/BRFSS_Field_Map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theresaszoke/Desktop/Classwork/diabetes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5EB7D2-213F-AF48-A036-B72EC244184D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398A3D7C-983C-AC44-9B69-9993F696E31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="740" windowWidth="29400" windowHeight="17260" activeTab="1" xr2:uid="{2BEC7167-3A60-5747-B803-1B5800393B56}"/>
+    <workbookView xWindow="-60" yWindow="740" windowWidth="29400" windowHeight="17260" activeTab="1" xr2:uid="{2BEC7167-3A60-5747-B803-1B5800393B56}"/>
   </bookViews>
   <sheets>
     <sheet name="Field Analysis" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="670">
   <si>
     <t>TOLDHI2</t>
   </si>
@@ -2048,6 +2048,9 @@
   </si>
   <si>
     <t>About how tall are you without shoes? (If respondent answers in metrics, put a 9 in the first column)[Round fractions down.] NOTE: we will use the field wtkg3 instead.</t>
+  </si>
+  <si>
+    <t>Adults who reported doing physical activity or exercise during the past 30 days other than their regular job</t>
   </si>
 </sst>
 </file>
@@ -2425,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AAFC5EA-9B3F-6E44-BC4E-3F13A83D01D0}">
   <dimension ref="A1:I455"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A67" sqref="A66:A67"/>
+    <sheetView topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="C295" sqref="C295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4225,7 +4228,7 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="4" t="s">
+      <c r="A66" t="s">
         <v>75</v>
       </c>
       <c r="B66" t="str">
@@ -4255,7 +4258,7 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A67" s="4" t="s">
+      <c r="A67" t="s">
         <v>76</v>
       </c>
       <c r="B67" t="str">
@@ -7401,7 +7404,7 @@
         <v>200</v>
       </c>
       <c r="B191" t="str">
-        <f t="shared" ref="B191:B222" si="24">VLOOKUP(A191,F:F,1,0)</f>
+        <f t="shared" ref="B191:B199" si="24">VLOOKUP(A191,F:F,1,0)</f>
         <v>LASTSIG3</v>
       </c>
       <c r="D191" t="s">
@@ -8490,7 +8493,7 @@
         <v>243</v>
       </c>
       <c r="B234" t="e">
-        <f t="shared" ref="B234:B265" si="29">VLOOKUP(A234,F:F,1,0)</f>
+        <f t="shared" ref="B234:B252" si="29">VLOOKUP(A234,F:F,1,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D234" t="s">
@@ -9041,7 +9044,7 @@
         <v>454</v>
       </c>
       <c r="G258" t="e">
-        <f t="shared" ref="G258:G321" si="31">VLOOKUP(F258,A:A,1,0)</f>
+        <f t="shared" ref="G258:G283" si="31">VLOOKUP(F258,A:A,1,0)</f>
         <v>#N/A</v>
       </c>
       <c r="I258" t="s">
@@ -9959,8 +9962,11 @@
         <f t="shared" si="34"/>
         <v>_TOTINDA</v>
       </c>
+      <c r="C295" t="s">
+        <v>669</v>
+      </c>
       <c r="D295" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="F295" t="s">
         <v>474</v>
@@ -10482,7 +10488,7 @@
         <v>320</v>
       </c>
       <c r="B318" t="e">
-        <f t="shared" ref="B318:B349" si="36">VLOOKUP(A318,F:F,1,0)</f>
+        <f t="shared" ref="B318:B331" si="36">VLOOKUP(A318,F:F,1,0)</f>
         <v>#N/A</v>
       </c>
       <c r="D318" t="s">
@@ -12035,13 +12041,12 @@
         <f t="shared" si="41"/>
         <v>_TOTINDA</v>
       </c>
-      <c r="H413">
+      <c r="H413" t="str">
         <f t="shared" si="42"/>
-        <v>0</v>
-      </c>
-      <c r="I413" t="str">
-        <f t="shared" si="43"/>
-        <v>drop</v>
+        <v>Adults who reported doing physical activity or exercise during the past 30 days other than their regular job</v>
+      </c>
+      <c r="I413" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="414" spans="6:9" x14ac:dyDescent="0.2">
@@ -12488,7 +12493,7 @@
         <v>276</v>
       </c>
       <c r="G446" t="str">
-        <f t="shared" ref="G446:G477" si="45">VLOOKUP(F446,A:A,1,0)</f>
+        <f t="shared" ref="G446:G455" si="45">VLOOKUP(F446,A:A,1,0)</f>
         <v>DRNKANY5</v>
       </c>
       <c r="H446">
@@ -12631,10 +12636,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F8025D-A42D-A644-ABEF-0A6D4C91F8C3}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13455,6 +13460,20 @@
         <v>662</v>
       </c>
       <c r="D57" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C58" t="s">
+        <v>669</v>
+      </c>
+      <c r="D58" t="s">
         <v>566</v>
       </c>
     </row>

</xml_diff>